<commit_message>
Iteration2: Precode, some code
</commit_message>
<xml_diff>
--- a/Iteration1/TimeLog-Iteration1.xlsx
+++ b/Iteration1/TimeLog-Iteration1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nil0310\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2FC3B4-A91D-4287-8135-CC5D5E3FD44D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{2D2FC3B4-A91D-4287-8135-CC5D5E3FD44D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{59E1655C-65DD-4118-A120-E07D4272993E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>PSP Time Recording Log</t>
   </si>
@@ -364,6 +364,81 @@
   </si>
   <si>
     <t>Start planning, project summary</t>
+  </si>
+  <si>
+    <t>1:20pm</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>1:45pm</t>
+  </si>
+  <si>
+    <t>2:25pm</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>3:20pm</t>
+  </si>
+  <si>
+    <t>3:24pm</t>
+  </si>
+  <si>
+    <t>Wrote the tests</t>
+  </si>
+  <si>
+    <t>Drew up class diagram</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>4:00pm</t>
+  </si>
+  <si>
+    <t>4:10pm</t>
+  </si>
+  <si>
+    <t>4:40pm</t>
+  </si>
+  <si>
+    <t>Wrote basic code, spike test, game logic</t>
+  </si>
+  <si>
+    <t>4:28pm</t>
+  </si>
+  <si>
+    <t>Test out functionality of written code</t>
+  </si>
+  <si>
+    <t>2:20pm</t>
+  </si>
+  <si>
+    <t>2:50pm</t>
+  </si>
+  <si>
+    <t>Break code up and follow MVC better</t>
+  </si>
+  <si>
+    <t>3:00pm</t>
+  </si>
+  <si>
+    <t>3:02pm</t>
+  </si>
+  <si>
+    <t>Test new code</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Never stopped</t>
+  </si>
+  <si>
+    <t>Post coding requirements (PIP, testing, writing more documentation)</t>
   </si>
 </sst>
 </file>
@@ -619,6 +694,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -634,8 +710,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,15 +1049,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
@@ -1047,20 +1122,142 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="14">
         <v>43548</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="14" t="s">
         <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="14">
+        <v>43548</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="14">
+        <v>43548</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="14">
+        <v>43548</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="14">
+        <v>43548</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="14">
+        <v>43549</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="14">
+        <v>43549</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="14">
+        <v>43549</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1089,7 +1286,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1097,31 +1294,31 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -1129,13 +1326,13 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
@@ -1165,7 +1362,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1173,13 +1370,13 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="10" t="s">
         <v>30</v>
       </c>

</xml_diff>